<commit_message>
Impresión de valores en reporte
</commit_message>
<xml_diff>
--- a/uploads/FORMATO_PAT.xlsx
+++ b/uploads/FORMATO_PAT.xlsx
@@ -1,20 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Planeacion\Evaluacion\DavidMoreno\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppServ\www\SIEVAL\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B4F0B5-A60B-4E9C-AC8F-C2E8CE4495D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PROGRAMACION" sheetId="11" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -186,7 +198,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -770,6 +785,33 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -804,12 +846,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -818,63 +854,6 @@
     <xf numFmtId="1" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -929,13 +908,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -962,6 +941,57 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1021,21 +1051,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1139,6 +1154,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1174,6 +1206,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1349,11 +1398,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:Y8"/>
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,395 +1435,395 @@
       <c r="A1" s="2"/>
     </row>
     <row r="2" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="89"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="89"/>
-      <c r="U2" s="89"/>
-      <c r="V2" s="89"/>
-      <c r="W2" s="89"/>
-      <c r="X2" s="89"/>
-      <c r="Y2" s="89"/>
+      <c r="A2" s="94"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="94"/>
+      <c r="M2" s="94"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="94"/>
+      <c r="Q2" s="94"/>
+      <c r="R2" s="94"/>
+      <c r="S2" s="94"/>
+      <c r="T2" s="94"/>
+      <c r="U2" s="94"/>
+      <c r="V2" s="94"/>
+      <c r="W2" s="94"/>
+      <c r="X2" s="94"/>
+      <c r="Y2" s="94"/>
     </row>
     <row r="3" spans="1:25" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="93" t="s">
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="L3" s="100"/>
-      <c r="M3" s="103"/>
-      <c r="N3" s="103"/>
-      <c r="O3" s="103"/>
-      <c r="P3" s="103"/>
-      <c r="Q3" s="103"/>
-      <c r="R3" s="103"/>
-      <c r="S3" s="103"/>
-      <c r="T3" s="103"/>
-      <c r="U3" s="103"/>
-      <c r="V3" s="103"/>
-      <c r="W3" s="104"/>
-      <c r="X3" s="37" t="s">
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="104" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="105"/>
+      <c r="M3" s="108"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="108"/>
+      <c r="P3" s="108"/>
+      <c r="Q3" s="108"/>
+      <c r="R3" s="108"/>
+      <c r="S3" s="108"/>
+      <c r="T3" s="108"/>
+      <c r="U3" s="108"/>
+      <c r="V3" s="108"/>
+      <c r="W3" s="109"/>
+      <c r="X3" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="Y3" s="38"/>
+      <c r="Y3" s="27"/>
     </row>
     <row r="4" spans="1:25" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="97"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="57" t="s">
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="101" t="s">
-        <v>0</v>
-      </c>
-      <c r="L4" s="102"/>
-      <c r="M4" s="107"/>
-      <c r="N4" s="108"/>
-      <c r="O4" s="108"/>
-      <c r="P4" s="108"/>
-      <c r="Q4" s="108"/>
-      <c r="R4" s="108"/>
-      <c r="S4" s="108"/>
-      <c r="T4" s="108"/>
-      <c r="U4" s="108"/>
-      <c r="V4" s="108"/>
-      <c r="W4" s="108"/>
-      <c r="X4" s="105"/>
-      <c r="Y4" s="106"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="107"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="113"/>
+      <c r="O4" s="113"/>
+      <c r="P4" s="113"/>
+      <c r="Q4" s="113"/>
+      <c r="R4" s="113"/>
+      <c r="S4" s="113"/>
+      <c r="T4" s="113"/>
+      <c r="U4" s="113"/>
+      <c r="V4" s="113"/>
+      <c r="W4" s="113"/>
+      <c r="X4" s="110"/>
+      <c r="Y4" s="111"/>
     </row>
     <row r="5" spans="1:25" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="57" t="s">
+      <c r="B5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="101" t="s">
-        <v>0</v>
-      </c>
-      <c r="L5" s="102"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="55"/>
-      <c r="O5" s="55"/>
-      <c r="P5" s="55"/>
-      <c r="Q5" s="55"/>
-      <c r="R5" s="55"/>
-      <c r="S5" s="55"/>
-      <c r="T5" s="55"/>
-      <c r="U5" s="55"/>
-      <c r="V5" s="55"/>
-      <c r="W5" s="55"/>
-      <c r="X5" s="105"/>
-      <c r="Y5" s="106"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="107"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="29"/>
+      <c r="X5" s="110"/>
+      <c r="Y5" s="111"/>
     </row>
     <row r="6" spans="1:25" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="66" t="s">
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="67"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="67"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="37" t="s">
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="53"/>
-      <c r="T6" s="53"/>
-      <c r="U6" s="53"/>
-      <c r="V6" s="53"/>
-      <c r="W6" s="53"/>
-      <c r="X6" s="53"/>
-      <c r="Y6" s="38"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="27"/>
     </row>
     <row r="7" spans="1:25" ht="74.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="63"/>
-      <c r="B7" s="64"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="54" t="s">
+      <c r="A7" s="51"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="N7" s="55"/>
-      <c r="O7" s="55"/>
-      <c r="P7" s="55"/>
-      <c r="Q7" s="55"/>
-      <c r="R7" s="55"/>
-      <c r="S7" s="55"/>
-      <c r="T7" s="55"/>
-      <c r="U7" s="55"/>
-      <c r="V7" s="55"/>
-      <c r="W7" s="55"/>
-      <c r="X7" s="55"/>
-      <c r="Y7" s="56"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="30"/>
     </row>
     <row r="8" spans="1:25" ht="74.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="57" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="58"/>
-      <c r="K8" s="58"/>
-      <c r="L8" s="58"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="58"/>
-      <c r="Q8" s="58"/>
-      <c r="R8" s="58"/>
-      <c r="S8" s="58"/>
-      <c r="T8" s="58"/>
-      <c r="U8" s="58"/>
-      <c r="V8" s="58"/>
-      <c r="W8" s="58"/>
-      <c r="X8" s="58"/>
-      <c r="Y8" s="59"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32"/>
+      <c r="T8" s="32"/>
+      <c r="U8" s="32"/>
+      <c r="V8" s="32"/>
+      <c r="W8" s="32"/>
+      <c r="X8" s="32"/>
+      <c r="Y8" s="33"/>
     </row>
     <row r="9" spans="1:25" ht="36.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="110"/>
-      <c r="C9" s="110"/>
-      <c r="D9" s="111"/>
-      <c r="E9" s="112" t="s">
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="112"/>
-      <c r="G9" s="112"/>
-      <c r="H9" s="112"/>
-      <c r="I9" s="112"/>
-      <c r="J9" s="112"/>
-      <c r="K9" s="112"/>
-      <c r="L9" s="112"/>
-      <c r="M9" s="112"/>
-      <c r="N9" s="112"/>
-      <c r="O9" s="112"/>
-      <c r="P9" s="112"/>
-      <c r="Q9" s="112"/>
-      <c r="R9" s="112"/>
-      <c r="S9" s="112"/>
-      <c r="T9" s="112"/>
-      <c r="U9" s="112"/>
-      <c r="V9" s="112"/>
-      <c r="W9" s="112"/>
-      <c r="X9" s="112"/>
-      <c r="Y9" s="113"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="80"/>
+      <c r="P9" s="80"/>
+      <c r="Q9" s="80"/>
+      <c r="R9" s="80"/>
+      <c r="S9" s="80"/>
+      <c r="T9" s="80"/>
+      <c r="U9" s="80"/>
+      <c r="V9" s="80"/>
+      <c r="W9" s="80"/>
+      <c r="X9" s="80"/>
+      <c r="Y9" s="81"/>
     </row>
     <row r="10" spans="1:25" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
       <c r="F10" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="31" t="s">
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="32"/>
-      <c r="S10" s="32"/>
-      <c r="T10" s="32"/>
-      <c r="U10" s="33"/>
-      <c r="V10" s="31" t="s">
+      <c r="P10" s="41"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="41"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="42"/>
+      <c r="V10" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="W10" s="32"/>
-      <c r="X10" s="32"/>
-      <c r="Y10" s="33"/>
+      <c r="W10" s="41"/>
+      <c r="X10" s="41"/>
+      <c r="Y10" s="42"/>
     </row>
     <row r="11" spans="1:25" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="70"/>
-      <c r="B11" s="72" t="s">
+      <c r="A11" s="58"/>
+      <c r="B11" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="78" t="s">
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="81" t="s">
+      <c r="G11" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="82"/>
-      <c r="I11" s="82"/>
-      <c r="J11" s="82"/>
-      <c r="K11" s="82"/>
-      <c r="L11" s="82"/>
-      <c r="M11" s="82"/>
-      <c r="N11" s="83"/>
-      <c r="O11" s="41"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="42"/>
-      <c r="S11" s="42"/>
-      <c r="T11" s="42"/>
-      <c r="U11" s="42"/>
-      <c r="V11" s="47" t="s">
+      <c r="H11" s="70"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="71"/>
+      <c r="O11" s="82"/>
+      <c r="P11" s="83"/>
+      <c r="Q11" s="83"/>
+      <c r="R11" s="83"/>
+      <c r="S11" s="83"/>
+      <c r="T11" s="83"/>
+      <c r="U11" s="83"/>
+      <c r="V11" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="W11" s="48"/>
-      <c r="X11" s="48"/>
-      <c r="Y11" s="49"/>
+      <c r="W11" s="89"/>
+      <c r="X11" s="89"/>
+      <c r="Y11" s="90"/>
     </row>
     <row r="12" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="71"/>
-      <c r="B12" s="72"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="73"/>
-      <c r="J12" s="73"/>
-      <c r="K12" s="73"/>
-      <c r="L12" s="73"/>
-      <c r="M12" s="73"/>
-      <c r="N12" s="84"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="44"/>
-      <c r="R12" s="44"/>
-      <c r="S12" s="44"/>
-      <c r="T12" s="44"/>
-      <c r="U12" s="44"/>
-      <c r="V12" s="47"/>
-      <c r="W12" s="48"/>
-      <c r="X12" s="48"/>
-      <c r="Y12" s="49"/>
+      <c r="A12" s="59"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="72"/>
+      <c r="O12" s="84"/>
+      <c r="P12" s="85"/>
+      <c r="Q12" s="85"/>
+      <c r="R12" s="85"/>
+      <c r="S12" s="85"/>
+      <c r="T12" s="85"/>
+      <c r="U12" s="85"/>
+      <c r="V12" s="88"/>
+      <c r="W12" s="89"/>
+      <c r="X12" s="89"/>
+      <c r="Y12" s="90"/>
     </row>
     <row r="13" spans="1:25" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="71"/>
-      <c r="B13" s="75"/>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="86"/>
-      <c r="L13" s="86"/>
-      <c r="M13" s="86"/>
-      <c r="N13" s="87"/>
-      <c r="O13" s="45"/>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="46"/>
-      <c r="S13" s="46"/>
-      <c r="T13" s="46"/>
-      <c r="U13" s="46"/>
-      <c r="V13" s="50"/>
-      <c r="W13" s="51"/>
-      <c r="X13" s="51"/>
-      <c r="Y13" s="52"/>
+      <c r="A13" s="59"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="74"/>
+      <c r="L13" s="74"/>
+      <c r="M13" s="74"/>
+      <c r="N13" s="75"/>
+      <c r="O13" s="86"/>
+      <c r="P13" s="87"/>
+      <c r="Q13" s="87"/>
+      <c r="R13" s="87"/>
+      <c r="S13" s="87"/>
+      <c r="T13" s="87"/>
+      <c r="U13" s="87"/>
+      <c r="V13" s="91"/>
+      <c r="W13" s="92"/>
+      <c r="X13" s="92"/>
+      <c r="Y13" s="93"/>
     </row>
     <row r="14" spans="1:25" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="35" t="s">
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="44" t="s">
         <v>47</v>
       </c>
       <c r="H14" s="12" t="s">
@@ -1819,19 +1868,19 @@
       <c r="W14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="X14" s="37" t="s">
+      <c r="X14" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="Y14" s="38"/>
+      <c r="Y14" s="27"/>
     </row>
     <row r="15" spans="1:25" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="36"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="45"/>
       <c r="H15" s="7">
         <v>0</v>
       </c>
@@ -1874,18 +1923,19 @@
       <c r="W15" s="7">
         <v>0</v>
       </c>
-      <c r="X15" s="39">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="40"/>
+      <c r="X15" s="46">
+        <f>SUM(H15:V15)</f>
+        <v>0</v>
+      </c>
+      <c r="Y15" s="47"/>
     </row>
     <row r="16" spans="1:25" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="31"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="33"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="42"/>
       <c r="G16" s="23" t="s">
         <v>48</v>
       </c>
@@ -1907,21 +1957,22 @@
       <c r="W16" s="7">
         <v>0</v>
       </c>
-      <c r="X16" s="39">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="40"/>
+      <c r="X16" s="46">
+        <f>SUM(H16:V16)</f>
+        <v>0</v>
+      </c>
+      <c r="Y16" s="47"/>
     </row>
     <row r="17" spans="1:27" ht="19.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="35" t="s">
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="44" t="s">
         <v>49</v>
       </c>
       <c r="H17" s="12" t="s">
@@ -1966,25 +2017,25 @@
       <c r="W17" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="X17" s="37" t="s">
+      <c r="X17" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="Y17" s="38"/>
+      <c r="Y17" s="27"/>
       <c r="Z17" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="AA17" s="34" t="s">
+      <c r="AA17" s="43" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="36"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="45"/>
       <c r="H18" s="7">
         <v>0</v>
       </c>
@@ -2027,22 +2078,23 @@
       <c r="W18" s="7">
         <v>0</v>
       </c>
-      <c r="X18" s="39">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="40"/>
+      <c r="X18" s="46">
+        <f>SUM(H18:V18)</f>
+        <v>0</v>
+      </c>
+      <c r="Y18" s="47"/>
       <c r="Z18" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AA18" s="34"/>
+      <c r="AA18" s="43"/>
     </row>
     <row r="19" spans="1:27" ht="19.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="31"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="42"/>
       <c r="G19" s="24" t="s">
         <v>50</v>
       </c>
@@ -2064,14 +2116,15 @@
       <c r="W19" s="7">
         <v>0</v>
       </c>
-      <c r="X19" s="39">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="40"/>
+      <c r="X19" s="46">
+        <f>SUM(H19:V19)</f>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="47"/>
       <c r="Z19" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="AA19" s="34"/>
+      <c r="AA19" s="43"/>
     </row>
     <row r="20" spans="1:27" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
@@ -2102,7 +2155,7 @@
       <c r="Z20" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="AA20" s="34"/>
+      <c r="AA20" s="43"/>
     </row>
     <row r="21" spans="1:27" ht="126.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
@@ -2183,12 +2236,15 @@
     <mergeCell ref="G21:J21"/>
     <mergeCell ref="M21:T21"/>
     <mergeCell ref="M22:T22"/>
+    <mergeCell ref="M4:W4"/>
     <mergeCell ref="V22:Y22"/>
     <mergeCell ref="V21:Y21"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="X14:Y14"/>
     <mergeCell ref="X15:Y15"/>
     <mergeCell ref="X16:Y16"/>
+    <mergeCell ref="O11:U13"/>
+    <mergeCell ref="V11:Y13"/>
     <mergeCell ref="A2:Y2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E5:J5"/>
@@ -2203,14 +2259,6 @@
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="X4:Y5"/>
     <mergeCell ref="E4:J4"/>
-    <mergeCell ref="M4:W4"/>
-    <mergeCell ref="A14:F16"/>
-    <mergeCell ref="A6:D7"/>
-    <mergeCell ref="E6:L7"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:N13"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="G10:N10"/>
     <mergeCell ref="A8:D8"/>
@@ -2218,8 +2266,6 @@
     <mergeCell ref="E9:Y9"/>
     <mergeCell ref="V10:Y10"/>
     <mergeCell ref="O10:U10"/>
-    <mergeCell ref="O11:U13"/>
-    <mergeCell ref="V11:Y13"/>
     <mergeCell ref="M6:Y6"/>
     <mergeCell ref="M7:Y7"/>
     <mergeCell ref="E8:Y8"/>
@@ -2229,6 +2275,13 @@
     <mergeCell ref="X17:Y17"/>
     <mergeCell ref="X18:Y18"/>
     <mergeCell ref="X19:Y19"/>
+    <mergeCell ref="A14:F16"/>
+    <mergeCell ref="A6:D7"/>
+    <mergeCell ref="E6:L7"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:N13"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.94488188976377963" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>